<commit_message>
ongoing testing work ... UserLoggerMiddleware passing, but FodyScopedLogger not writing to file during method Entry/Exit -- using MinimumLevel from config
</commit_message>
<xml_diff>
--- a/test/MiddlewareTests/MiddlewareTests/UserLogger/TestJson.xlsx
+++ b/test/MiddlewareTests/MiddlewareTests/UserLogger/TestJson.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denmi\source\repos\EDennis.AspNetCore.Base\test\MiddlewareTests\MiddlewareTests\UserLogger\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MitchellDenC\source\repos\EDennis.AspNetCore.Base\test\MiddlewareTests\MiddlewareTests\UserLogger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7D9142-84EC-4A7C-A0CE-DAF8757DE67D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571DB4A9-0E64-4D35-A5C7-8EEB942A211C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="17993" windowHeight="10800" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
+    <workbookView xWindow="25080" yWindow="255" windowWidth="25440" windowHeight="15390" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="30">
   <si>
     <t>ProjectName</t>
   </si>
@@ -81,39 +81,21 @@
     <t>Information</t>
   </si>
   <si>
-    <t>v=0</t>
-  </si>
-  <si>
     <t>QueryString1</t>
   </si>
   <si>
     <t>QueryString2</t>
   </si>
   <si>
-    <t>X-Clear-ScopedLogger=moe</t>
-  </si>
-  <si>
-    <t>X-Set-ScopedLogger=larry|Debug</t>
-  </si>
-  <si>
-    <t>X-Clear-ScopedLogger=larry</t>
-  </si>
-  <si>
     <t>X-User=curly&amp;X-Set-ScopedLogger=curly|Information</t>
   </si>
   <si>
-    <t>X-Clear-ScopedLogger=curly</t>
-  </si>
-  <si>
     <t>Expected1</t>
   </si>
   <si>
     <t>Expected2</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>QueryString3</t>
   </si>
   <si>
@@ -124,6 +106,21 @@
   </si>
   <si>
     <t>X-User=shemp</t>
+  </si>
+  <si>
+    <t>header*X-User=moe&amp;header*X-Set-ScopedLogger=moe|Trace</t>
+  </si>
+  <si>
+    <t>header*X-User=larry&amp;X-Set-ScopedLogger=larry|Debug</t>
+  </si>
+  <si>
+    <t>header*X-User=moe&amp;X-Clear-ScopedLogger=moe</t>
+  </si>
+  <si>
+    <t>header*X-User=larry&amp;X-Clear-ScopedLogger=larry</t>
+  </si>
+  <si>
+    <t>X-User=curly&amp;X-Clear-ScopedLogger=curly</t>
   </si>
 </sst>
 </file>
@@ -478,23 +475,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DF70F6-41B8-4967-A575-80BF52770920}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.59765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.86328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.59765625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1328125" style="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="42.73046875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="1" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="42.7109375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,7 +514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -531,13 +528,13 @@
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -551,13 +548,13 @@
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -571,13 +568,13 @@
         <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -591,13 +588,13 @@
         <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -611,13 +608,13 @@
         <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -631,13 +628,13 @@
         <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -651,13 +648,13 @@
         <v>8</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -671,13 +668,13 @@
         <v>8</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -691,13 +688,13 @@
         <v>8</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -711,13 +708,13 @@
         <v>8</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -731,13 +728,13 @@
         <v>8</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -751,13 +748,13 @@
         <v>8</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -771,13 +768,13 @@
         <v>10</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -791,13 +788,13 @@
         <v>10</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -811,13 +808,13 @@
         <v>10</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -831,13 +828,13 @@
         <v>10</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -851,13 +848,13 @@
         <v>10</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -871,10 +868,10 @@
         <v>10</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>